<commit_message>
removed copyright to avoid politics
</commit_message>
<xml_diff>
--- a/public/ValueSet-ConsentExchangePolicies.xlsx
+++ b/public/ValueSet-ConsentExchangePolicies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Property</t>
   </si>
@@ -55,7 +55,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-09T09:51:53-05:00</t>
+    <t>2024-09-09T14:48:24-05:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -67,7 +67,13 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>MITRE, Inc (https://github.com/awatson1978/us-state-profiles)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -92,9 +98,6 @@
   </si>
   <si>
     <t>All codes</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>System URI</t>
@@ -228,10 +231,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -240,7 +243,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -340,20 +343,28 @@
       <c r="A12" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>21</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s" s="2">
         <v>23</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -375,28 +386,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -418,12 +429,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>